<commit_message>
feat: adicionado script que normaliza a tabela unificada, preparando para receber algoritmos de ml
</commit_message>
<xml_diff>
--- a/alunos_unificado.xlsx
+++ b/alunos_unificado.xlsx
@@ -42599,7 +42599,7 @@
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D862" t="n">
@@ -43481,7 +43481,7 @@
       </c>
       <c r="C880" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D880" t="n">
@@ -44069,7 +44069,7 @@
       </c>
       <c r="C892" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D892" t="n">
@@ -44118,7 +44118,7 @@
       </c>
       <c r="C893" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D893" t="n">
@@ -44167,7 +44167,7 @@
       </c>
       <c r="C894" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D894" t="n">
@@ -44216,7 +44216,7 @@
       </c>
       <c r="C895" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D895" t="n">
@@ -44265,7 +44265,7 @@
       </c>
       <c r="C896" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D896" t="n">
@@ -44314,7 +44314,7 @@
       </c>
       <c r="C897" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D897" t="n">
@@ -44363,7 +44363,7 @@
       </c>
       <c r="C898" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D898" t="n">
@@ -44412,7 +44412,7 @@
       </c>
       <c r="C899" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D899" t="n">
@@ -44461,7 +44461,7 @@
       </c>
       <c r="C900" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D900" t="n">
@@ -44510,7 +44510,7 @@
       </c>
       <c r="C901" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D901" t="n">
@@ -44559,7 +44559,7 @@
       </c>
       <c r="C902" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D902" t="n">
@@ -44608,7 +44608,7 @@
       </c>
       <c r="C903" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D903" t="n">
@@ -44657,7 +44657,7 @@
       </c>
       <c r="C904" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D904" t="n">
@@ -44706,7 +44706,7 @@
       </c>
       <c r="C905" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D905" t="n">
@@ -44755,7 +44755,7 @@
       </c>
       <c r="C906" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D906" t="n">
@@ -44804,7 +44804,7 @@
       </c>
       <c r="C907" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D907" t="n">
@@ -44951,7 +44951,7 @@
       </c>
       <c r="C910" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D910" t="n">
@@ -45000,7 +45000,7 @@
       </c>
       <c r="C911" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D911" t="n">
@@ -45049,7 +45049,7 @@
       </c>
       <c r="C912" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D912" t="n">
@@ -45098,7 +45098,7 @@
       </c>
       <c r="C913" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D913" t="n">
@@ -45147,7 +45147,7 @@
       </c>
       <c r="C914" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D914" t="n">
@@ -45294,7 +45294,7 @@
       </c>
       <c r="C917" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D917" t="n">
@@ -45833,7 +45833,7 @@
       </c>
       <c r="C928" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D928" t="n">
@@ -47001,7 +47001,7 @@
       </c>
       <c r="C952" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D952" t="n">
@@ -48324,7 +48324,7 @@
       </c>
       <c r="C979" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D979" t="n">
@@ -48716,7 +48716,7 @@
       </c>
       <c r="C987" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D987" t="n">
@@ -49545,7 +49545,7 @@
       </c>
       <c r="C1004" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D1004" t="n">
@@ -49594,7 +49594,7 @@
       </c>
       <c r="C1005" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D1005" t="n">
@@ -91477,7 +91477,7 @@
       </c>
       <c r="C1860" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D1860" t="n">
@@ -91624,7 +91624,7 @@
       </c>
       <c r="C1863" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Escola Pública</t>
         </is>
       </c>
       <c r="D1863" t="n">

</xml_diff>